<commit_message>
feat: update new excel template
</commit_message>
<xml_diff>
--- a/public/qs-survey-recommenders-template.xlsx
+++ b/public/qs-survey-recommenders-template.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB59267-22EA-45B2-9D92-8D0574B227A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAF2157-1C50-43D4-93AB-1AC68B4D8F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="填寫說明" sheetId="1" r:id="rId1"/>
     <sheet name="聲譽調查提名名冊-學界" sheetId="2" r:id="rId2"/>
     <sheet name="聲譽調查提名名冊-業界" sheetId="4" r:id="rId3"/>
-    <sheet name="工作表1" sheetId="6" state="hidden" r:id="rId4"/>
-    <sheet name="工作表3" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="產業別【中英對照表】" sheetId="7" state="hidden" r:id="rId4"/>
+    <sheet name="工作表1" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="工作表3" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="369">
   <si>
     <r>
       <t xml:space="preserve">Title
@@ -183,6 +184,1547 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>QS業界領域別</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounting &amp; Finance </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agriculture &amp; Forestry</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Anatomy &amp; Physiology </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Anthropology </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Archaeology </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Architecture &amp; Built</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Area Studies </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Art &amp; Design </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Astronomy </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Biological Sciences </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Business &amp; Management Studies</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chemistry</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classics &amp; Ancient History</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication &amp; Media Studies </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Science &amp; Info Systems </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Dentistry </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Development Studies </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth Sciences </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Economics &amp; Econometrics </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Education Social</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Engineering </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">English Language &amp; Literature </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental Sciences </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">European studies </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Food Science &amp; Technology </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Genetics &amp; Biotechnology </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geography</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">History </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hospitality &amp; Leisure Management</t>
+  </si>
+  <si>
+    <t>International Affairs</t>
+  </si>
+  <si>
+    <t>Law</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Library &amp; Information Management</t>
+  </si>
+  <si>
+    <t>Linguistics</t>
+  </si>
+  <si>
+    <t>Marine Sciences</t>
+  </si>
+  <si>
+    <t>Environment Marketing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Materials Science</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Modern Languages</t>
+  </si>
+  <si>
+    <t>Music</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nursing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Performing Arts</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pharmacology</t>
+  </si>
+  <si>
+    <t>Pharmacy</t>
+  </si>
+  <si>
+    <t>Philosophy</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Politics</t>
+  </si>
+  <si>
+    <t>Psychology</t>
+  </si>
+  <si>
+    <t>Policy &amp; Administration</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Social Work</t>
+  </si>
+  <si>
+    <t>Sociology</t>
+  </si>
+  <si>
+    <t>Sports-related Subjects</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statistics &amp; Operational Research</t>
+  </si>
+  <si>
+    <t>Theology, Divinity &amp; Religious Studies</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Veterinary Science</t>
+  </si>
+  <si>
+    <t>Any Discipline</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Position
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>職稱</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Position
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>職稱</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Department
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>所屬系所</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>單位名</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Institution Name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>所屬學校</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>機構名</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>稱謂</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">First Name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>名字</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Last Name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>姓氏</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Company Name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>所屬公司</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>機構名</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Location
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>所處國別</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>通訊電郵</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Industry
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>產業別</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>下拉式選單</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提供此名單之教師姓名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提供此名單提供之教師通訊電郵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Aland Islands</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
+    <t>Antarctica</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Bonaire, Sint Eustatius and Saba</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Bouvet Island</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>British Indian Ocean Territory</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Christmas Island</t>
+  </si>
+  <si>
+    <t>Cocos (Keeling) Islands</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Congo, Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Cook Islands</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Cote D'Ivoire</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Falkland Islands (Malvinas)</t>
+  </si>
+  <si>
+    <t>Faroe Islands</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>French Guiana</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
+  </si>
+  <si>
+    <t>French Southern Territories</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Guadeloupe</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guernsey</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Heard Island and Mcdonald Islands</t>
+  </si>
+  <si>
+    <t>Holy See (Vatican City State)</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iran, Islamic Republic of</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Isle of Man</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>Korea, Democratic People's Republic of</t>
+  </si>
+  <si>
+    <t>Korea, Republic of</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Libyan Arab Jamahiriya</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Macao</t>
+  </si>
+  <si>
+    <t>Macedonia, the Former Yugoslav Republic of</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Martinique</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Mayotte</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Micronesia, Federated States of</t>
+  </si>
+  <si>
+    <t>Moldova, Republic of</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Montserrat</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Netherlands Antilles</t>
+  </si>
+  <si>
+    <t>New Caledonia</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Niue</t>
+  </si>
+  <si>
+    <t>Norfolk Island</t>
+  </si>
+  <si>
+    <t>Northern Mariana Islands</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>Palestinian Territory, Occupied</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Pitcairn</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Reunion</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saint Barthelemy</t>
+  </si>
+  <si>
+    <t>Saint Helena</t>
+  </si>
+  <si>
+    <t>Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Saint Martin</t>
+  </si>
+  <si>
+    <t>Saint Pierre and Miquelon</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Serbia and Montenegro</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Sint Maarten</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>South Georgia and the South Sandwich Islands</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Svalbard and Jan Mayen</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Tokelau</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>United States Minor Outlying Islands</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>Virgin Islands, British</t>
+  </si>
+  <si>
+    <t>Virgin Islands, U.s.</t>
+  </si>
+  <si>
+    <t>Wallis and Futuna</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanzania</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Location
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>所處國別</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agriculture, Forestry, Fishing and Animal Husbandry</t>
+  </si>
+  <si>
+    <t>Mining and Quarrying</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Electricity and Gas Supply</t>
+  </si>
+  <si>
+    <t>Water Supply and Remediation Activities</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Wholesale and Retail Trade</t>
+  </si>
+  <si>
+    <t>Transportation and Storage</t>
+  </si>
+  <si>
+    <t>Accommodation and Food Service Activities</t>
+  </si>
+  <si>
+    <t>Information and Communication</t>
+  </si>
+  <si>
+    <t>Financial and Insurance Activities</t>
+  </si>
+  <si>
+    <t>Real Estate Activities</t>
+  </si>
+  <si>
+    <t>Professional, Scientific and Technical Activities</t>
+  </si>
+  <si>
+    <t>Support Service Activities</t>
+  </si>
+  <si>
+    <t>Public Administration and Defence</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Human Health and Social Work Activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arts, Entertainment and Recreation </t>
+  </si>
+  <si>
+    <t>Other Service Activities</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Industry  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>產業別</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>農、林、漁、牧業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>礦業及土石採取業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>製造業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>電力及燃氣供應業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>用水供應及污染整治業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>營造業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>批發及零售業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>運輸及倉儲業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>住宿及餐飲業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資訊及通訊傳播業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>金融及保險業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>不動產業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>專業、科學及技術服務業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>支援服務業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>公共行政及國防</t>
+    </r>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>教育服務業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>醫療保健及社會工作服務業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>藝術、娛樂及休閒服務業</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>其他服務業</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -424,7 +1966,19 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>其他人員亦可列上，但建議以以上三項資格者為優先。</t>
+      <t xml:space="preserve">其他人員亦可列上，但建議以以上三項資格者為優先。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">(產業別【中英對照】可參考右方表格)
+</t>
     </r>
     <r>
       <rPr>
@@ -815,1263 +2369,6 @@
         <charset val="136"/>
       </rPr>
       <t>3675</t>
-    </r>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QS業界領域別</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Accounting &amp; Finance </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Agriculture &amp; Forestry</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Anatomy &amp; Physiology </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Anthropology </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Archaeology </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Architecture &amp; Built</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Area Studies </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Art &amp; Design </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Astronomy </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Biological Sciences </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Business &amp; Management Studies</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chemistry</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Classics &amp; Ancient History</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Communication &amp; Media Studies </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer Science &amp; Info Systems </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Dentistry </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Development Studies </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Earth Sciences </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Economics &amp; Econometrics </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Education Social</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Engineering </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">English Language &amp; Literature </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Environmental Sciences </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">European studies </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Food Science &amp; Technology </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Genetics &amp; Biotechnology </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geography</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">History </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hospitality &amp; Leisure Management</t>
-  </si>
-  <si>
-    <t>International Affairs</t>
-  </si>
-  <si>
-    <t>Law</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Library &amp; Information Management</t>
-  </si>
-  <si>
-    <t>Linguistics</t>
-  </si>
-  <si>
-    <t>Marine Sciences</t>
-  </si>
-  <si>
-    <t>Environment Marketing</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Materials Science</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
-    <t>Medicine</t>
-  </si>
-  <si>
-    <t>Modern Languages</t>
-  </si>
-  <si>
-    <t>Music</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nursing</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Performing Arts</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pharmacology</t>
-  </si>
-  <si>
-    <t>Pharmacy</t>
-  </si>
-  <si>
-    <t>Philosophy</t>
-  </si>
-  <si>
-    <t>Physics</t>
-  </si>
-  <si>
-    <t>Politics</t>
-  </si>
-  <si>
-    <t>Psychology</t>
-  </si>
-  <si>
-    <t>Policy &amp; Administration</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Social Work</t>
-  </si>
-  <si>
-    <t>Sociology</t>
-  </si>
-  <si>
-    <t>Sports-related Subjects</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Statistics &amp; Operational Research</t>
-  </si>
-  <si>
-    <t>Theology, Divinity &amp; Religious Studies</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Veterinary Science</t>
-  </si>
-  <si>
-    <t>Any Discipline</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Position
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>職稱</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Position
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>職稱</t>
-    </r>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Department
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>所屬系所</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>單位名</t>
-    </r>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Institution Name
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>所屬學校</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>機構名</t>
-    </r>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Title
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>稱謂</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">First Name
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>名字</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Last Name
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>姓氏</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Company Name
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>所屬公司</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>機構名</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Location
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>所處國別</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Email
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>通訊電郵</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Industry
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>產業別</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>下拉式選單</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提供此名單之教師姓名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提供此名單提供之教師通訊電郵</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Afghanistan</t>
-  </si>
-  <si>
-    <t>Aland Islands</t>
-  </si>
-  <si>
-    <t>Albania</t>
-  </si>
-  <si>
-    <t>Algeria</t>
-  </si>
-  <si>
-    <t>American Samoa</t>
-  </si>
-  <si>
-    <t>Andorra</t>
-  </si>
-  <si>
-    <t>Angola</t>
-  </si>
-  <si>
-    <t>Anguilla</t>
-  </si>
-  <si>
-    <t>Antarctica</t>
-  </si>
-  <si>
-    <t>Antigua and Barbuda</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Armenia</t>
-  </si>
-  <si>
-    <t>Aruba</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Azerbaijan</t>
-  </si>
-  <si>
-    <t>Bahamas</t>
-  </si>
-  <si>
-    <t>Bahrain</t>
-  </si>
-  <si>
-    <t>Bangladesh</t>
-  </si>
-  <si>
-    <t>Barbados</t>
-  </si>
-  <si>
-    <t>Belarus</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Belize</t>
-  </si>
-  <si>
-    <t>Benin</t>
-  </si>
-  <si>
-    <t>Bermuda</t>
-  </si>
-  <si>
-    <t>Bhutan</t>
-  </si>
-  <si>
-    <t>Bolivia</t>
-  </si>
-  <si>
-    <t>Bonaire, Sint Eustatius and Saba</t>
-  </si>
-  <si>
-    <t>Bosnia and Herzegovina</t>
-  </si>
-  <si>
-    <t>Botswana</t>
-  </si>
-  <si>
-    <t>Bouvet Island</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>British Indian Ocean Territory</t>
-  </si>
-  <si>
-    <t>Brunei Darussalam</t>
-  </si>
-  <si>
-    <t>Bulgaria</t>
-  </si>
-  <si>
-    <t>Burkina Faso</t>
-  </si>
-  <si>
-    <t>Burundi</t>
-  </si>
-  <si>
-    <t>Cambodia</t>
-  </si>
-  <si>
-    <t>Cameroon</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Cape Verde</t>
-  </si>
-  <si>
-    <t>Cayman Islands</t>
-  </si>
-  <si>
-    <t>Central African Republic</t>
-  </si>
-  <si>
-    <t>Chad</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Christmas Island</t>
-  </si>
-  <si>
-    <t>Cocos (Keeling) Islands</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>Comoros</t>
-  </si>
-  <si>
-    <t>Congo</t>
-  </si>
-  <si>
-    <t>Congo, Democratic Republic of the Congo</t>
-  </si>
-  <si>
-    <t>Cook Islands</t>
-  </si>
-  <si>
-    <t>Costa Rica</t>
-  </si>
-  <si>
-    <t>Cote D'Ivoire</t>
-  </si>
-  <si>
-    <t>Croatia</t>
-  </si>
-  <si>
-    <t>Cuba</t>
-  </si>
-  <si>
-    <t>Curacao</t>
-  </si>
-  <si>
-    <t>Cyprus</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Djibouti</t>
-  </si>
-  <si>
-    <t>Dominica</t>
-  </si>
-  <si>
-    <t>Dominican Republic</t>
-  </si>
-  <si>
-    <t>Ecuador</t>
-  </si>
-  <si>
-    <t>Egypt</t>
-  </si>
-  <si>
-    <t>El Salvador</t>
-  </si>
-  <si>
-    <t>Equatorial Guinea</t>
-  </si>
-  <si>
-    <t>Eritrea</t>
-  </si>
-  <si>
-    <t>Estonia</t>
-  </si>
-  <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
-    <t>Falkland Islands (Malvinas)</t>
-  </si>
-  <si>
-    <t>Faroe Islands</t>
-  </si>
-  <si>
-    <t>Fiji</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>French Guiana</t>
-  </si>
-  <si>
-    <t>French Polynesia</t>
-  </si>
-  <si>
-    <t>French Southern Territories</t>
-  </si>
-  <si>
-    <t>Gabon</t>
-  </si>
-  <si>
-    <t>Gambia</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Ghana</t>
-  </si>
-  <si>
-    <t>Gibraltar</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Greenland</t>
-  </si>
-  <si>
-    <t>Grenada</t>
-  </si>
-  <si>
-    <t>Guadeloupe</t>
-  </si>
-  <si>
-    <t>Guam</t>
-  </si>
-  <si>
-    <t>Guatemala</t>
-  </si>
-  <si>
-    <t>Guernsey</t>
-  </si>
-  <si>
-    <t>Guinea</t>
-  </si>
-  <si>
-    <t>Guinea-Bissau</t>
-  </si>
-  <si>
-    <t>Guyana</t>
-  </si>
-  <si>
-    <t>Haiti</t>
-  </si>
-  <si>
-    <t>Heard Island and Mcdonald Islands</t>
-  </si>
-  <si>
-    <t>Holy See (Vatican City State)</t>
-  </si>
-  <si>
-    <t>Honduras</t>
-  </si>
-  <si>
-    <t>Hong Kong</t>
-  </si>
-  <si>
-    <t>Hungary</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>Iran, Islamic Republic of</t>
-  </si>
-  <si>
-    <t>Iraq</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Isle of Man</t>
-  </si>
-  <si>
-    <t>Israel</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Jamaica</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Jersey</t>
-  </si>
-  <si>
-    <t>Jordan</t>
-  </si>
-  <si>
-    <t>Kazakhstan</t>
-  </si>
-  <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>Kiribati</t>
-  </si>
-  <si>
-    <t>Korea, Democratic People's Republic of</t>
-  </si>
-  <si>
-    <t>Korea, Republic of</t>
-  </si>
-  <si>
-    <t>Kosovo</t>
-  </si>
-  <si>
-    <t>Kuwait</t>
-  </si>
-  <si>
-    <t>Kyrgyzstan</t>
-  </si>
-  <si>
-    <t>Lao People's Democratic Republic</t>
-  </si>
-  <si>
-    <t>Latvia</t>
-  </si>
-  <si>
-    <t>Lebanon</t>
-  </si>
-  <si>
-    <t>Lesotho</t>
-  </si>
-  <si>
-    <t>Liberia</t>
-  </si>
-  <si>
-    <t>Libyan Arab Jamahiriya</t>
-  </si>
-  <si>
-    <t>Liechtenstein</t>
-  </si>
-  <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>Luxembourg</t>
-  </si>
-  <si>
-    <t>Macao</t>
-  </si>
-  <si>
-    <t>Macedonia, the Former Yugoslav Republic of</t>
-  </si>
-  <si>
-    <t>Madagascar</t>
-  </si>
-  <si>
-    <t>Malawi</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>Maldives</t>
-  </si>
-  <si>
-    <t>Mali</t>
-  </si>
-  <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>Marshall Islands</t>
-  </si>
-  <si>
-    <t>Martinique</t>
-  </si>
-  <si>
-    <t>Mauritania</t>
-  </si>
-  <si>
-    <t>Mauritius</t>
-  </si>
-  <si>
-    <t>Mayotte</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Micronesia, Federated States of</t>
-  </si>
-  <si>
-    <t>Moldova, Republic of</t>
-  </si>
-  <si>
-    <t>Monaco</t>
-  </si>
-  <si>
-    <t>Mongolia</t>
-  </si>
-  <si>
-    <t>Montenegro</t>
-  </si>
-  <si>
-    <t>Montserrat</t>
-  </si>
-  <si>
-    <t>Morocco</t>
-  </si>
-  <si>
-    <t>Mozambique</t>
-  </si>
-  <si>
-    <t>Myanmar</t>
-  </si>
-  <si>
-    <t>Namibia</t>
-  </si>
-  <si>
-    <t>Nauru</t>
-  </si>
-  <si>
-    <t>Nepal</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Netherlands Antilles</t>
-  </si>
-  <si>
-    <t>New Caledonia</t>
-  </si>
-  <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
-    <t>Nicaragua</t>
-  </si>
-  <si>
-    <t>Niger</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>Niue</t>
-  </si>
-  <si>
-    <t>Norfolk Island</t>
-  </si>
-  <si>
-    <t>Northern Mariana Islands</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Oman</t>
-  </si>
-  <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
-    <t>Palau</t>
-  </si>
-  <si>
-    <t>Palestinian Territory, Occupied</t>
-  </si>
-  <si>
-    <t>Panama</t>
-  </si>
-  <si>
-    <t>Papua New Guinea</t>
-  </si>
-  <si>
-    <t>Paraguay</t>
-  </si>
-  <si>
-    <t>Peru</t>
-  </si>
-  <si>
-    <t>Philippines</t>
-  </si>
-  <si>
-    <t>Pitcairn</t>
-  </si>
-  <si>
-    <t>Poland</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Puerto Rico</t>
-  </si>
-  <si>
-    <t>Qatar</t>
-  </si>
-  <si>
-    <t>Reunion</t>
-  </si>
-  <si>
-    <t>Romania</t>
-  </si>
-  <si>
-    <t>Russian Federation</t>
-  </si>
-  <si>
-    <t>Rwanda</t>
-  </si>
-  <si>
-    <t>Saint Barthelemy</t>
-  </si>
-  <si>
-    <t>Saint Helena</t>
-  </si>
-  <si>
-    <t>Saint Kitts and Nevis</t>
-  </si>
-  <si>
-    <t>Saint Lucia</t>
-  </si>
-  <si>
-    <t>Saint Martin</t>
-  </si>
-  <si>
-    <t>Saint Pierre and Miquelon</t>
-  </si>
-  <si>
-    <t>Saint Vincent and the Grenadines</t>
-  </si>
-  <si>
-    <t>Samoa</t>
-  </si>
-  <si>
-    <t>San Marino</t>
-  </si>
-  <si>
-    <t>Sao Tome and Principe</t>
-  </si>
-  <si>
-    <t>Saudi Arabia</t>
-  </si>
-  <si>
-    <t>Senegal</t>
-  </si>
-  <si>
-    <t>Serbia</t>
-  </si>
-  <si>
-    <t>Serbia and Montenegro</t>
-  </si>
-  <si>
-    <t>Seychelles</t>
-  </si>
-  <si>
-    <t>Sierra Leone</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>Sint Maarten</t>
-  </si>
-  <si>
-    <t>Slovakia</t>
-  </si>
-  <si>
-    <t>Slovenia</t>
-  </si>
-  <si>
-    <t>Solomon Islands</t>
-  </si>
-  <si>
-    <t>Somalia</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>South Georgia and the South Sandwich Islands</t>
-  </si>
-  <si>
-    <t>South Sudan</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Sri Lanka</t>
-  </si>
-  <si>
-    <t>Sudan</t>
-  </si>
-  <si>
-    <t>Suriname</t>
-  </si>
-  <si>
-    <t>Svalbard and Jan Mayen</t>
-  </si>
-  <si>
-    <t>Swaziland</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>Syrian Arab Republic</t>
-  </si>
-  <si>
-    <t>Tajikistan</t>
-  </si>
-  <si>
-    <t>Thailand</t>
-  </si>
-  <si>
-    <t>Timor-Leste</t>
-  </si>
-  <si>
-    <t>Togo</t>
-  </si>
-  <si>
-    <t>Tokelau</t>
-  </si>
-  <si>
-    <t>Tonga</t>
-  </si>
-  <si>
-    <t>Trinidad and Tobago</t>
-  </si>
-  <si>
-    <t>Tunisia</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
-    <t>Turkmenistan</t>
-  </si>
-  <si>
-    <t>Turks and Caicos Islands</t>
-  </si>
-  <si>
-    <t>Tuvalu</t>
-  </si>
-  <si>
-    <t>Uganda</t>
-  </si>
-  <si>
-    <t>Ukraine</t>
-  </si>
-  <si>
-    <t>United Arab Emirates</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>United States Minor Outlying Islands</t>
-  </si>
-  <si>
-    <t>Uruguay</t>
-  </si>
-  <si>
-    <t>Uzbekistan</t>
-  </si>
-  <si>
-    <t>Vanuatu</t>
-  </si>
-  <si>
-    <t>Venezuela</t>
-  </si>
-  <si>
-    <t>Viet Nam</t>
-  </si>
-  <si>
-    <t>Virgin Islands, British</t>
-  </si>
-  <si>
-    <t>Virgin Islands, U.s.</t>
-  </si>
-  <si>
-    <t>Wallis and Futuna</t>
-  </si>
-  <si>
-    <t>Western Sahara</t>
-  </si>
-  <si>
-    <t>Yemen</t>
-  </si>
-  <si>
-    <t>Zambia</t>
-  </si>
-  <si>
-    <t>Zimbabwe</t>
-  </si>
-  <si>
-    <t>Taiwan</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tanzania</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Location
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>所處國別</t>
     </r>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2080,7 +2377,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2355,6 +2652,17 @@
       <color rgb="FF000000"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
     </font>
   </fonts>
@@ -2801,7 +3109,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2844,14 +3152,21 @@
     <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2909,6 +3224,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3800475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="圖片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60858FAC-404D-4D9B-A4A5-73D6B83F3362}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8848725" y="28575"/>
+          <a:ext cx="5591175" cy="4010025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3174,10 +3555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3192,42 +3573,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="9" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="A2" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A9:F9"/>
+  <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
   </mergeCells>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="37" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3264,10 +3637,10 @@
     </row>
     <row r="2" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
@@ -3279,16 +3652,16 @@
         <v>3</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="I2" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>2</v>
@@ -3351,34 +3724,34 @@
     </row>
     <row r="2" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="C2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -3389,18 +3762,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5337837A-E763-493C-8177-718A09A8971D}">
           <x14:formula1>
             <xm:f>工作表3!$A$2:$A$58</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G1048576</xm:sqref>
+          <xm:sqref>G342:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AE16C18-18E0-49DB-A535-AAA19EB61937}">
           <x14:formula1>
             <xm:f>工作表1!$A$3:$IR$3</xm:f>
           </x14:formula1>
           <xm:sqref>I3:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{978AD899-BE74-4BBF-9D64-691EA161B9BE}">
+          <x14:formula1>
+            <xm:f>產業別【中英對照表】!$B$3:$B$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>G3:G341</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3409,6 +3788,187 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F73F962-8556-42E7-9EF9-552D4FD523A2}">
+  <dimension ref="A2:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="18"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5AF902-A1E8-4FC6-A31D-C9CD744A2D1C}">
   <dimension ref="A3:IR3"/>
   <sheetViews>
@@ -3420,760 +3980,760 @@
   <sheetData>
     <row r="3" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>79</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>80</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>82</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>83</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>84</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>85</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>86</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>87</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>88</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>89</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>90</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>91</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>92</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>93</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>94</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>95</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>96</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>97</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>98</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>99</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>100</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>101</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>102</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>103</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>104</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>106</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>107</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>108</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>109</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>110</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>111</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>112</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>113</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>114</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>115</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>116</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>117</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>118</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AR3" t="s">
         <v>119</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AS3" t="s">
         <v>120</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AT3" t="s">
         <v>121</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AU3" t="s">
         <v>122</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AV3" t="s">
         <v>123</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AW3" t="s">
         <v>124</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AX3" t="s">
         <v>125</v>
       </c>
-      <c r="AX3" t="s">
+      <c r="AY3" t="s">
         <v>126</v>
       </c>
-      <c r="AY3" t="s">
+      <c r="AZ3" t="s">
         <v>127</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BA3" t="s">
         <v>128</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BB3" t="s">
         <v>129</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BC3" t="s">
         <v>130</v>
       </c>
-      <c r="BC3" t="s">
+      <c r="BD3" t="s">
         <v>131</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BE3" t="s">
         <v>132</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BF3" t="s">
         <v>133</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BG3" t="s">
         <v>134</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BH3" t="s">
         <v>135</v>
       </c>
-      <c r="BH3" t="s">
+      <c r="BI3" t="s">
         <v>136</v>
       </c>
-      <c r="BI3" t="s">
+      <c r="BJ3" t="s">
         <v>137</v>
       </c>
-      <c r="BJ3" t="s">
+      <c r="BK3" t="s">
         <v>138</v>
       </c>
-      <c r="BK3" t="s">
+      <c r="BL3" t="s">
         <v>139</v>
       </c>
-      <c r="BL3" t="s">
+      <c r="BM3" t="s">
         <v>140</v>
       </c>
-      <c r="BM3" t="s">
+      <c r="BN3" t="s">
         <v>141</v>
       </c>
-      <c r="BN3" t="s">
+      <c r="BO3" t="s">
         <v>142</v>
       </c>
-      <c r="BO3" t="s">
+      <c r="BP3" t="s">
         <v>143</v>
       </c>
-      <c r="BP3" t="s">
+      <c r="BQ3" t="s">
         <v>144</v>
       </c>
-      <c r="BQ3" t="s">
+      <c r="BR3" t="s">
         <v>145</v>
       </c>
-      <c r="BR3" t="s">
+      <c r="BS3" t="s">
         <v>146</v>
       </c>
-      <c r="BS3" t="s">
+      <c r="BT3" t="s">
         <v>147</v>
       </c>
-      <c r="BT3" t="s">
+      <c r="BU3" t="s">
         <v>148</v>
       </c>
-      <c r="BU3" t="s">
+      <c r="BV3" t="s">
         <v>149</v>
       </c>
-      <c r="BV3" t="s">
+      <c r="BW3" t="s">
         <v>150</v>
       </c>
-      <c r="BW3" t="s">
+      <c r="BX3" t="s">
         <v>151</v>
       </c>
-      <c r="BX3" t="s">
+      <c r="BY3" t="s">
         <v>152</v>
       </c>
-      <c r="BY3" t="s">
+      <c r="BZ3" t="s">
         <v>153</v>
       </c>
-      <c r="BZ3" t="s">
+      <c r="CA3" t="s">
         <v>154</v>
       </c>
-      <c r="CA3" t="s">
+      <c r="CB3" t="s">
         <v>155</v>
       </c>
-      <c r="CB3" t="s">
+      <c r="CC3" t="s">
         <v>156</v>
       </c>
-      <c r="CC3" t="s">
+      <c r="CD3" t="s">
         <v>157</v>
       </c>
-      <c r="CD3" t="s">
+      <c r="CE3" t="s">
         <v>158</v>
       </c>
-      <c r="CE3" t="s">
+      <c r="CF3" t="s">
         <v>159</v>
       </c>
-      <c r="CF3" t="s">
+      <c r="CG3" t="s">
         <v>160</v>
       </c>
-      <c r="CG3" t="s">
+      <c r="CH3" t="s">
         <v>161</v>
       </c>
-      <c r="CH3" t="s">
+      <c r="CI3" t="s">
         <v>162</v>
       </c>
-      <c r="CI3" t="s">
+      <c r="CJ3" t="s">
         <v>163</v>
       </c>
-      <c r="CJ3" t="s">
+      <c r="CK3" t="s">
         <v>164</v>
       </c>
-      <c r="CK3" t="s">
+      <c r="CL3" t="s">
         <v>165</v>
       </c>
-      <c r="CL3" t="s">
+      <c r="CM3" t="s">
         <v>166</v>
       </c>
-      <c r="CM3" t="s">
+      <c r="CN3" t="s">
         <v>167</v>
       </c>
-      <c r="CN3" t="s">
+      <c r="CO3" t="s">
         <v>168</v>
       </c>
-      <c r="CO3" t="s">
+      <c r="CP3" t="s">
         <v>169</v>
       </c>
-      <c r="CP3" t="s">
+      <c r="CQ3" t="s">
         <v>170</v>
       </c>
-      <c r="CQ3" t="s">
+      <c r="CR3" t="s">
         <v>171</v>
       </c>
-      <c r="CR3" t="s">
+      <c r="CS3" t="s">
         <v>172</v>
       </c>
-      <c r="CS3" t="s">
+      <c r="CT3" t="s">
         <v>173</v>
       </c>
-      <c r="CT3" t="s">
+      <c r="CU3" t="s">
         <v>174</v>
       </c>
-      <c r="CU3" t="s">
+      <c r="CV3" t="s">
         <v>175</v>
       </c>
-      <c r="CV3" t="s">
+      <c r="CW3" t="s">
         <v>176</v>
       </c>
-      <c r="CW3" t="s">
+      <c r="CX3" t="s">
         <v>177</v>
       </c>
-      <c r="CX3" t="s">
+      <c r="CY3" t="s">
         <v>178</v>
       </c>
-      <c r="CY3" t="s">
+      <c r="CZ3" t="s">
         <v>179</v>
       </c>
-      <c r="CZ3" t="s">
+      <c r="DA3" t="s">
         <v>180</v>
       </c>
-      <c r="DA3" t="s">
+      <c r="DB3" t="s">
         <v>181</v>
       </c>
-      <c r="DB3" t="s">
+      <c r="DC3" t="s">
         <v>182</v>
       </c>
-      <c r="DC3" t="s">
+      <c r="DD3" t="s">
         <v>183</v>
       </c>
-      <c r="DD3" t="s">
+      <c r="DE3" t="s">
         <v>184</v>
       </c>
-      <c r="DE3" t="s">
+      <c r="DF3" t="s">
         <v>185</v>
       </c>
-      <c r="DF3" t="s">
+      <c r="DG3" t="s">
         <v>186</v>
       </c>
-      <c r="DG3" t="s">
+      <c r="DH3" t="s">
         <v>187</v>
       </c>
-      <c r="DH3" t="s">
+      <c r="DI3" t="s">
         <v>188</v>
       </c>
-      <c r="DI3" t="s">
+      <c r="DJ3" t="s">
         <v>189</v>
       </c>
-      <c r="DJ3" t="s">
+      <c r="DK3" t="s">
         <v>190</v>
       </c>
-      <c r="DK3" t="s">
+      <c r="DL3" t="s">
         <v>191</v>
       </c>
-      <c r="DL3" t="s">
+      <c r="DM3" t="s">
         <v>192</v>
       </c>
-      <c r="DM3" t="s">
+      <c r="DN3" t="s">
         <v>193</v>
       </c>
-      <c r="DN3" t="s">
+      <c r="DO3" t="s">
         <v>194</v>
       </c>
-      <c r="DO3" t="s">
+      <c r="DP3" t="s">
         <v>195</v>
       </c>
-      <c r="DP3" t="s">
+      <c r="DQ3" t="s">
         <v>196</v>
       </c>
-      <c r="DQ3" t="s">
+      <c r="DR3" t="s">
         <v>197</v>
       </c>
-      <c r="DR3" t="s">
+      <c r="DS3" t="s">
         <v>198</v>
       </c>
-      <c r="DS3" t="s">
+      <c r="DT3" t="s">
         <v>199</v>
       </c>
-      <c r="DT3" t="s">
+      <c r="DU3" t="s">
         <v>200</v>
       </c>
-      <c r="DU3" t="s">
+      <c r="DV3" t="s">
         <v>201</v>
       </c>
-      <c r="DV3" t="s">
+      <c r="DW3" t="s">
         <v>202</v>
       </c>
-      <c r="DW3" t="s">
+      <c r="DX3" t="s">
         <v>203</v>
       </c>
-      <c r="DX3" t="s">
+      <c r="DY3" t="s">
         <v>204</v>
       </c>
-      <c r="DY3" t="s">
+      <c r="DZ3" t="s">
         <v>205</v>
       </c>
-      <c r="DZ3" t="s">
+      <c r="EA3" t="s">
         <v>206</v>
       </c>
-      <c r="EA3" t="s">
+      <c r="EB3" t="s">
         <v>207</v>
       </c>
-      <c r="EB3" t="s">
+      <c r="EC3" t="s">
         <v>208</v>
       </c>
-      <c r="EC3" t="s">
+      <c r="ED3" t="s">
         <v>209</v>
       </c>
-      <c r="ED3" t="s">
+      <c r="EE3" t="s">
         <v>210</v>
       </c>
-      <c r="EE3" t="s">
+      <c r="EF3" t="s">
         <v>211</v>
       </c>
-      <c r="EF3" t="s">
+      <c r="EG3" t="s">
         <v>212</v>
       </c>
-      <c r="EG3" t="s">
+      <c r="EH3" t="s">
         <v>213</v>
       </c>
-      <c r="EH3" t="s">
+      <c r="EI3" t="s">
         <v>214</v>
       </c>
-      <c r="EI3" t="s">
+      <c r="EJ3" t="s">
         <v>215</v>
       </c>
-      <c r="EJ3" t="s">
+      <c r="EK3" t="s">
         <v>216</v>
       </c>
-      <c r="EK3" t="s">
+      <c r="EL3" t="s">
         <v>217</v>
       </c>
-      <c r="EL3" t="s">
+      <c r="EM3" t="s">
         <v>218</v>
       </c>
-      <c r="EM3" t="s">
+      <c r="EN3" t="s">
         <v>219</v>
       </c>
-      <c r="EN3" t="s">
+      <c r="EO3" t="s">
         <v>220</v>
       </c>
-      <c r="EO3" t="s">
+      <c r="EP3" t="s">
         <v>221</v>
       </c>
-      <c r="EP3" t="s">
+      <c r="EQ3" t="s">
         <v>222</v>
       </c>
-      <c r="EQ3" t="s">
+      <c r="ER3" t="s">
         <v>223</v>
       </c>
-      <c r="ER3" t="s">
+      <c r="ES3" t="s">
         <v>224</v>
       </c>
-      <c r="ES3" t="s">
+      <c r="ET3" t="s">
         <v>225</v>
       </c>
-      <c r="ET3" t="s">
+      <c r="EU3" t="s">
         <v>226</v>
       </c>
-      <c r="EU3" t="s">
+      <c r="EV3" t="s">
         <v>227</v>
       </c>
-      <c r="EV3" t="s">
+      <c r="EW3" t="s">
         <v>228</v>
       </c>
-      <c r="EW3" t="s">
+      <c r="EX3" t="s">
         <v>229</v>
       </c>
-      <c r="EX3" t="s">
+      <c r="EY3" t="s">
         <v>230</v>
       </c>
-      <c r="EY3" t="s">
+      <c r="EZ3" t="s">
         <v>231</v>
       </c>
-      <c r="EZ3" t="s">
+      <c r="FA3" t="s">
         <v>232</v>
       </c>
-      <c r="FA3" t="s">
+      <c r="FB3" t="s">
         <v>233</v>
       </c>
-      <c r="FB3" t="s">
+      <c r="FC3" t="s">
         <v>234</v>
       </c>
-      <c r="FC3" t="s">
+      <c r="FD3" t="s">
         <v>235</v>
       </c>
-      <c r="FD3" t="s">
+      <c r="FE3" t="s">
         <v>236</v>
       </c>
-      <c r="FE3" t="s">
+      <c r="FF3" t="s">
         <v>237</v>
       </c>
-      <c r="FF3" t="s">
+      <c r="FG3" t="s">
         <v>238</v>
       </c>
-      <c r="FG3" t="s">
+      <c r="FH3" t="s">
         <v>239</v>
       </c>
-      <c r="FH3" t="s">
+      <c r="FI3" t="s">
         <v>240</v>
       </c>
-      <c r="FI3" t="s">
+      <c r="FJ3" t="s">
         <v>241</v>
       </c>
-      <c r="FJ3" t="s">
+      <c r="FK3" t="s">
         <v>242</v>
       </c>
-      <c r="FK3" t="s">
+      <c r="FL3" t="s">
         <v>243</v>
       </c>
-      <c r="FL3" t="s">
+      <c r="FM3" t="s">
         <v>244</v>
       </c>
-      <c r="FM3" t="s">
+      <c r="FN3" t="s">
         <v>245</v>
       </c>
-      <c r="FN3" t="s">
+      <c r="FO3" t="s">
         <v>246</v>
       </c>
-      <c r="FO3" t="s">
+      <c r="FP3" t="s">
         <v>247</v>
       </c>
-      <c r="FP3" t="s">
+      <c r="FQ3" t="s">
         <v>248</v>
       </c>
-      <c r="FQ3" t="s">
+      <c r="FR3" t="s">
         <v>249</v>
       </c>
-      <c r="FR3" t="s">
+      <c r="FS3" t="s">
         <v>250</v>
       </c>
-      <c r="FS3" t="s">
+      <c r="FT3" t="s">
         <v>251</v>
       </c>
-      <c r="FT3" t="s">
+      <c r="FU3" t="s">
         <v>252</v>
       </c>
-      <c r="FU3" t="s">
+      <c r="FV3" t="s">
         <v>253</v>
       </c>
-      <c r="FV3" t="s">
+      <c r="FW3" t="s">
         <v>254</v>
       </c>
-      <c r="FW3" t="s">
+      <c r="FX3" t="s">
         <v>255</v>
       </c>
-      <c r="FX3" t="s">
+      <c r="FY3" t="s">
         <v>256</v>
       </c>
-      <c r="FY3" t="s">
+      <c r="FZ3" t="s">
         <v>257</v>
       </c>
-      <c r="FZ3" t="s">
+      <c r="GA3" t="s">
         <v>258</v>
       </c>
-      <c r="GA3" t="s">
+      <c r="GB3" t="s">
         <v>259</v>
       </c>
-      <c r="GB3" t="s">
+      <c r="GC3" t="s">
         <v>260</v>
       </c>
-      <c r="GC3" t="s">
+      <c r="GD3" t="s">
         <v>261</v>
       </c>
-      <c r="GD3" t="s">
+      <c r="GE3" t="s">
         <v>262</v>
       </c>
-      <c r="GE3" t="s">
+      <c r="GF3" t="s">
         <v>263</v>
       </c>
-      <c r="GF3" t="s">
+      <c r="GG3" t="s">
         <v>264</v>
       </c>
-      <c r="GG3" t="s">
+      <c r="GH3" t="s">
         <v>265</v>
       </c>
-      <c r="GH3" t="s">
+      <c r="GI3" t="s">
         <v>266</v>
       </c>
-      <c r="GI3" t="s">
+      <c r="GJ3" t="s">
         <v>267</v>
       </c>
-      <c r="GJ3" t="s">
+      <c r="GK3" t="s">
         <v>268</v>
       </c>
-      <c r="GK3" t="s">
+      <c r="GL3" t="s">
         <v>269</v>
       </c>
-      <c r="GL3" t="s">
+      <c r="GM3" t="s">
         <v>270</v>
       </c>
-      <c r="GM3" t="s">
+      <c r="GN3" t="s">
         <v>271</v>
       </c>
-      <c r="GN3" t="s">
+      <c r="GO3" t="s">
         <v>272</v>
       </c>
-      <c r="GO3" t="s">
+      <c r="GP3" t="s">
         <v>273</v>
       </c>
-      <c r="GP3" t="s">
+      <c r="GQ3" t="s">
         <v>274</v>
       </c>
-      <c r="GQ3" t="s">
+      <c r="GR3" t="s">
         <v>275</v>
       </c>
-      <c r="GR3" t="s">
+      <c r="GS3" t="s">
         <v>276</v>
       </c>
-      <c r="GS3" t="s">
+      <c r="GT3" t="s">
         <v>277</v>
       </c>
-      <c r="GT3" t="s">
+      <c r="GU3" t="s">
         <v>278</v>
       </c>
-      <c r="GU3" t="s">
+      <c r="GV3" t="s">
         <v>279</v>
       </c>
-      <c r="GV3" t="s">
+      <c r="GW3" t="s">
         <v>280</v>
       </c>
-      <c r="GW3" t="s">
+      <c r="GX3" t="s">
         <v>281</v>
       </c>
-      <c r="GX3" t="s">
+      <c r="GY3" t="s">
         <v>282</v>
       </c>
-      <c r="GY3" t="s">
+      <c r="GZ3" t="s">
         <v>283</v>
       </c>
-      <c r="GZ3" t="s">
+      <c r="HA3" t="s">
         <v>284</v>
       </c>
-      <c r="HA3" t="s">
+      <c r="HB3" t="s">
         <v>285</v>
       </c>
-      <c r="HB3" t="s">
+      <c r="HC3" t="s">
         <v>286</v>
       </c>
-      <c r="HC3" t="s">
+      <c r="HD3" t="s">
         <v>287</v>
       </c>
-      <c r="HD3" t="s">
+      <c r="HE3" t="s">
         <v>288</v>
       </c>
-      <c r="HE3" t="s">
+      <c r="HF3" t="s">
         <v>289</v>
       </c>
-      <c r="HF3" t="s">
+      <c r="HG3" t="s">
         <v>290</v>
       </c>
-      <c r="HG3" t="s">
+      <c r="HH3" t="s">
         <v>291</v>
       </c>
-      <c r="HH3" t="s">
+      <c r="HI3" t="s">
         <v>292</v>
       </c>
-      <c r="HI3" t="s">
+      <c r="HJ3" t="s">
         <v>293</v>
       </c>
-      <c r="HJ3" t="s">
+      <c r="HK3" t="s">
         <v>294</v>
       </c>
-      <c r="HK3" t="s">
+      <c r="HL3" t="s">
         <v>295</v>
       </c>
-      <c r="HL3" t="s">
+      <c r="HM3" t="s">
+        <v>326</v>
+      </c>
+      <c r="HN3" t="s">
         <v>296</v>
       </c>
-      <c r="HM3" t="s">
+      <c r="HO3" t="s">
         <v>327</v>
       </c>
-      <c r="HN3" t="s">
+      <c r="HP3" t="s">
         <v>297</v>
       </c>
-      <c r="HO3" t="s">
-        <v>328</v>
-      </c>
-      <c r="HP3" t="s">
+      <c r="HQ3" t="s">
         <v>298</v>
       </c>
-      <c r="HQ3" t="s">
+      <c r="HR3" t="s">
         <v>299</v>
       </c>
-      <c r="HR3" t="s">
+      <c r="HS3" t="s">
         <v>300</v>
       </c>
-      <c r="HS3" t="s">
+      <c r="HT3" t="s">
         <v>301</v>
       </c>
-      <c r="HT3" t="s">
+      <c r="HU3" t="s">
         <v>302</v>
       </c>
-      <c r="HU3" t="s">
+      <c r="HV3" t="s">
         <v>303</v>
       </c>
-      <c r="HV3" t="s">
+      <c r="HW3" t="s">
         <v>304</v>
       </c>
-      <c r="HW3" t="s">
+      <c r="HX3" t="s">
         <v>305</v>
       </c>
-      <c r="HX3" t="s">
+      <c r="HY3" t="s">
         <v>306</v>
       </c>
-      <c r="HY3" t="s">
+      <c r="HZ3" t="s">
         <v>307</v>
       </c>
-      <c r="HZ3" t="s">
+      <c r="IA3" t="s">
         <v>308</v>
       </c>
-      <c r="IA3" t="s">
+      <c r="IB3" t="s">
         <v>309</v>
       </c>
-      <c r="IB3" t="s">
+      <c r="IC3" t="s">
         <v>310</v>
       </c>
-      <c r="IC3" t="s">
+      <c r="ID3" t="s">
         <v>311</v>
       </c>
-      <c r="ID3" t="s">
+      <c r="IE3" t="s">
         <v>312</v>
       </c>
-      <c r="IE3" t="s">
+      <c r="IF3" t="s">
         <v>313</v>
       </c>
-      <c r="IF3" t="s">
+      <c r="IG3" t="s">
         <v>314</v>
       </c>
-      <c r="IG3" t="s">
+      <c r="IH3" t="s">
         <v>315</v>
       </c>
-      <c r="IH3" t="s">
+      <c r="II3" t="s">
         <v>316</v>
       </c>
-      <c r="II3" t="s">
+      <c r="IJ3" t="s">
         <v>317</v>
       </c>
-      <c r="IJ3" t="s">
+      <c r="IK3" t="s">
         <v>318</v>
       </c>
-      <c r="IK3" t="s">
+      <c r="IL3" t="s">
         <v>319</v>
       </c>
-      <c r="IL3" t="s">
+      <c r="IM3" t="s">
         <v>320</v>
       </c>
-      <c r="IM3" t="s">
+      <c r="IN3" t="s">
         <v>321</v>
       </c>
-      <c r="IN3" t="s">
+      <c r="IO3" t="s">
         <v>322</v>
       </c>
-      <c r="IO3" t="s">
+      <c r="IP3" t="s">
         <v>323</v>
       </c>
-      <c r="IP3" t="s">
+      <c r="IQ3" t="s">
         <v>324</v>
       </c>
-      <c r="IQ3" t="s">
+      <c r="IR3" t="s">
         <v>325</v>
-      </c>
-      <c r="IR3" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4183,7 +4743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2522C696-34B4-42D7-8963-2BC5DDB7C06B}">
   <dimension ref="A1:A58"/>
   <sheetViews>
@@ -4198,287 +4758,287 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>